<commit_message>
the most statisfying result ever
</commit_message>
<xml_diff>
--- a/src/cellphonedb/excels/edge_list/top_cluster_interactions_15.xlsx
+++ b/src/cellphonedb/excels/edge_list/top_cluster_interactions_15.xlsx
@@ -468,19 +468,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Neu.Epend.0, MeV.Endothelial.2</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>MeV.Fib.4</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>15</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Neu.Epend.0, MeV.Endothelial.2</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -491,19 +491,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>MeV.FibCollagen.2</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>MeV.Endothelial.0</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>9</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>MeV.FibCollagen.2</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -514,19 +514,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>MeV.Endothelial.1, MeV.Endothelial.2</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>MeV.Endothelial.1, MeV.Pericytes.0, MeV.FibCollagen.2</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="E4" t="n">
         <v>9</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>MeV.Endothelial.1, MeV.Endothelial.2</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -537,19 +537,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Imm.PVM.0, MeV.FibCollagen.2</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>MeV.FibCollagen.2</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="E5" t="n">
         <v>11</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Imm.PVM.0, MeV.FibCollagen.2</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -560,19 +560,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Neu.Epend.0</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>MeV.Fib.5, MeV.FibCollagen.3</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="E6" t="n">
         <v>13</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Neu.Epend.0</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -583,19 +583,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Imm.DAM.0, Imm.DAM.1</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>MeV.FibCollagen.1</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="E7" t="n">
         <v>11</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Imm.DAM.0, Imm.DAM.1</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -606,19 +606,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Imm.Interferon.0, MeV.FibCollagen.1</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>Imm.PVM.0, MeV.Fib.5</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="E8" t="n">
         <v>11</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Imm.Interferon.0, MeV.FibCollagen.1</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -629,7 +629,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MeV.FibCollagen.3, Imm.Interferon.0</t>
+          <t>Imm.DAM.0</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -637,7 +637,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Imm.DAM.0</t>
+          <t>MeV.FibCollagen.3, Imm.Interferon.0</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -652,19 +652,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Imm.DAM.0</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>15</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>MeV.FibCollagen.3</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="E10" t="n">
         <v>11</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Imm.DAM.0</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -675,19 +675,19 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>MeV.FibCollagen.3</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>17</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>MeV.Pericytes.0</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="E11" t="n">
         <v>11</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>MeV.FibCollagen.3</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -698,19 +698,19 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>MeV.FibCollagen.3</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>18</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>MeV.Fib.5</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="E12" t="n">
         <v>15</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>MeV.FibCollagen.3</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -721,19 +721,19 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>MeV.Pericytes.0</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>13</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>Imm.DAM.1</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="E13" t="n">
         <v>8</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>MeV.Pericytes.0</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -744,19 +744,19 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Imm.PVM.0</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>MeV.FibCollagen.1</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="E14" t="n">
         <v>18</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Imm.PVM.0</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -767,19 +767,19 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>MeV.Pericytes.0</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>12</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>MeV.FibCollagen.1</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="E15" t="n">
         <v>17</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>MeV.Pericytes.0</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -790,19 +790,19 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Imm.DAM.0</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>13</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>Imm.PVM.0</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="E16" t="n">
         <v>14</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Imm.DAM.0</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
order of cluster in heatmaps
</commit_message>
<xml_diff>
--- a/src/cellphonedb/excels/edge_list/top_cluster_interactions_15.xlsx
+++ b/src/cellphonedb/excels/edge_list/top_cluster_interactions_15.xlsx
@@ -22,13 +22,13 @@
     <t>Top Sender(s)</t>
   </si>
   <si>
+    <t>Max Outgoing Interactions</t>
+  </si>
+  <si>
+    <t>Top Receiver(s)</t>
+  </si>
+  <si>
     <t>Max Incoming Interactions</t>
-  </si>
-  <si>
-    <t>Top Receiver(s)</t>
-  </si>
-  <si>
-    <t>Max Outgoing Interactions</t>
   </si>
   <si>
     <t>Imm.DAM.0</t>

</xml_diff>